<commit_message>
English speaking countries filter, top9 data frame/top 3 countries.
</commit_message>
<xml_diff>
--- a/Data/Investments.xlsx
+++ b/Data/Investments.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chiranjeev\Documents\Investment case study Cohort-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Annamalai Ganapathy\Documents\DSGroupProject\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F50F418-E518-4337-8312-B77483F9A775}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7080" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>C1</t>
   </si>
@@ -357,12 +358,34 @@
   </si>
   <si>
     <t>Sector-wise Investment Analysis</t>
+  </si>
+  <si>
+    <t>Venture Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+66368</t>
+  </si>
+  <si>
+    <t>permalink</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Great Britan</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -573,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -632,47 +655,53 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -987,11 +1016,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,23 +1031,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -1031,14 +1060,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>1</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="37" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
@@ -1047,7 +1078,9 @@
       <c r="B6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="17"/>
+      <c r="C6" s="36">
+        <v>66368</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -1056,7 +1089,9 @@
       <c r="B7" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="36" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -1065,7 +1100,9 @@
       <c r="B8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="36" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
@@ -1074,7 +1111,9 @@
       <c r="B9" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="36">
+        <v>114949</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="11"/>
@@ -1102,11 +1141,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,21 +1156,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
     </row>
     <row r="3" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -1151,7 +1190,9 @@
       <c r="B5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="12">
+        <v>11748949.130000001</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
@@ -1160,7 +1201,9 @@
       <c r="B6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="12">
+        <v>958694.47</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
@@ -1169,7 +1212,9 @@
       <c r="B7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="12">
+        <v>719818</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
@@ -1178,7 +1223,9 @@
       <c r="B8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="12">
+        <v>73308593.030000001</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
@@ -1187,7 +1234,9 @@
       <c r="B9" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="12" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1210,11 +1259,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,21 +1274,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
     </row>
     <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -1259,7 +1308,9 @@
       <c r="B5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
@@ -1268,7 +1319,9 @@
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
@@ -1277,7 +1330,9 @@
       <c r="B7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1299,11 +1354,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1316,38 +1371,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="30"/>
+      <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="24" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Python - final cleanup.
</commit_message>
<xml_diff>
--- a/Data/Investments.xlsx
+++ b/Data/Investments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Annamalai Ganapathy\Documents\DSGroupProject\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3935DA-CC1C-4025-BD3C-1C177309119A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C1E9DE-19A8-468D-A6CC-A4588FEC33B9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7080" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="51">
   <si>
     <t>C1</t>
   </si>
@@ -614,7 +614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -722,6 +722,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1039,7 +1040,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1287,7 +1288,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1382,7 +1383,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1458,7 +1459,7 @@
       <c r="D6" s="17">
         <v>2787592073</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="39">
         <v>1521271777</v>
       </c>
     </row>

</xml_diff>